<commit_message>
se incorpora proveedor a ingreso masivo
</commit_message>
<xml_diff>
--- a/public/documentos/documento_ejemplo.xlsx
+++ b/public/documentos/documento_ejemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\desarrollo\public\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FC40DE2-EAAE-43A9-8E7D-ACDB4220BC7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB18678-E75A-4374-9764-C8BE4F927273}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{864B328B-6E13-4141-A69F-4D95903D2F75}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>valor_producto</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Charger</t>
+  </si>
+  <si>
+    <t>datapro</t>
+  </si>
+  <si>
+    <t>nombre_proveedor</t>
   </si>
 </sst>
 </file>
@@ -138,9 +144,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D179583-4827-441A-B862-12DC4FFDABBE}" name="Tabla1" displayName="Tabla1" ref="A1:H3" totalsRowShown="0">
-  <autoFilter ref="A1:H3" xr:uid="{06BD64EC-342A-4FDB-893B-2057C080607F}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D179583-4827-441A-B862-12DC4FFDABBE}" name="Tabla1" displayName="Tabla1" ref="A1:I3" totalsRowShown="0">
+  <autoFilter ref="A1:I3" xr:uid="{06BD64EC-342A-4FDB-893B-2057C080607F}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{CC24F511-9C99-4FBA-9F1E-1B43FD35C2DD}" name="valor_producto" dataDxfId="0">
       <calculatedColumnFormula>ROUND((((Tabla1[[#This Row],[margen]]/100)*Tabla1[[#This Row],[costo]])+Tabla1[[#This Row],[costo]]),0)</calculatedColumnFormula>
     </tableColumn>
@@ -151,6 +157,7 @@
     <tableColumn id="7" xr3:uid="{A5228463-515E-4746-89DA-61D74B8E50E8}" name="stock"/>
     <tableColumn id="8" xr3:uid="{CE1D4515-9ABA-4A9E-A7B9-EF45A5698951}" name="costo"/>
     <tableColumn id="9" xr3:uid="{B22D76CD-6597-4735-AA73-6401D2A565F8}" name="margen"/>
+    <tableColumn id="4" xr3:uid="{E1034A79-4584-4E1F-837A-48FC6A3CF4C0}" name="nombre_proveedor"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -453,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E24082-6067-4761-9EF3-BBEA5EB05779}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,9 +473,10 @@
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,8 +501,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>ROUND((((Tabla1[[#This Row],[margen]]/100)*Tabla1[[#This Row],[costo]])+Tabla1[[#This Row],[costo]]),0)</f>
         <v>150</v>
@@ -520,8 +531,11 @@
       <c r="H2">
         <v>50</v>
       </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>ROUND((((Tabla1[[#This Row],[margen]]/100)*Tabla1[[#This Row],[costo]])+Tabla1[[#This Row],[costo]]),0)</f>
         <v>63</v>
@@ -547,8 +561,11 @@
       <c r="H3">
         <v>25</v>
       </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
     </row>
   </sheetData>

</xml_diff>